<commit_message>
tests lcga + divide pipeline in 3
</commit_message>
<xml_diff>
--- a/test/benchmark_lcga/algo_evaluation_lcga.xlsx
+++ b/test/benchmark_lcga/algo_evaluation_lcga.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Desktop\3A\Stage3A\longitudinalmodels\test\benchmark_lcga\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B896237-C147-4DF4-B357-28A9ABACA344}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E324CCBD-24C6-4BAF-BFEE-C6944ED181B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="28">
   <si>
     <t>same value as ground-truth</t>
   </si>
@@ -64,21 +64,12 @@
     <t>degree</t>
   </si>
   <si>
-    <t>betas ok</t>
-  </si>
-  <si>
-    <t>Rs ok</t>
-  </si>
-  <si>
     <t>ok</t>
   </si>
   <si>
     <t>not ok</t>
   </si>
   <si>
-    <t>pis ok</t>
-  </si>
-  <si>
     <t>almost</t>
   </si>
   <si>
@@ -92,6 +83,65 @@
   </si>
   <si>
     <t>0,.5,1,1.5</t>
+  </si>
+  <si>
+    <t>Rs ok (flexmix)</t>
+  </si>
+  <si>
+    <t>pis ok (flexmix)</t>
+  </si>
+  <si>
+    <t>betas ok (flexmix)</t>
+  </si>
+  <si>
+    <t>betas ok (custom flexmix)</t>
+  </si>
+  <si>
+    <t>Rs ok custom flexmix)</t>
+  </si>
+  <si>
+    <t>pis ok (custom flexmix)</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">in our simulation, some iterations found a result very close to flexmix, but duer to mulststart the final output is different, which corroborates that our algorithm was </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>better</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> than flexmix in this dataset</t>
+    </r>
+  </si>
+  <si>
+    <t>needed to rerun flexmix to have same res!</t>
+  </si>
+  <si>
+    <t>almost (3 cases)</t>
+  </si>
+  <si>
+    <t>almost (4 cases)</t>
   </si>
 </sst>
 </file>
@@ -171,7 +221,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -181,6 +231,9 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -461,19 +514,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3FF2FA4-DDBE-4CE0-8905-B56226955A6C}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="10.33203125" customWidth="1"/>
-    <col min="5" max="5" width="13.77734375" customWidth="1"/>
+    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="43.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>6</v>
       </c>
@@ -484,19 +543,31 @@
         <v>8</v>
       </c>
       <c r="D1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>10</v>
-      </c>
       <c r="G1" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
         <v>5</v>
       </c>
@@ -507,19 +578,28 @@
         <v>1</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>6</v>
       </c>
@@ -530,19 +610,31 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="H3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>7</v>
       </c>
@@ -553,19 +645,28 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="H4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="63.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>8</v>
       </c>
@@ -576,19 +677,31 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+      <c r="H5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>9</v>
       </c>
@@ -599,16 +712,25 @@
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G6" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="H6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6" t="s">
+        <v>26</v>
+      </c>
+      <c r="J6" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tests lcga using wsl
</commit_message>
<xml_diff>
--- a/test/benchmark_lcga/algo_evaluation_lcga.xlsx
+++ b/test/benchmark_lcga/algo_evaluation_lcga.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Desktop\3A\Stage3A\longitudinalmodels\test\benchmark_lcga\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E324CCBD-24C6-4BAF-BFEE-C6944ED181B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4288C5EC-7F20-492D-85E6-357E58919D85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="31">
   <si>
     <t>same value as ground-truth</t>
   </si>
@@ -143,12 +143,42 @@
   <si>
     <t>almost (4 cases)</t>
   </si>
+  <si>
+    <t>class-wise optimisation in M-step</t>
+  </si>
+  <si>
+    <t>Weighted Least Squares per class in M-step (equivalent to MLE)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(3 cases for </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>σ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, 2 for σ^2)</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -163,6 +193,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -221,7 +257,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -233,6 +269,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -514,10 +553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3FF2FA4-DDBE-4CE0-8905-B56226955A6C}">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -568,110 +607,94 @@
       </c>
     </row>
     <row r="2" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="8">
+      <c r="A2" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="8">
         <v>5</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B3" s="8">
         <v>2</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C3" s="8">
         <v>1</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="8" t="s">
+      <c r="E3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>6</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I3" t="s">
-        <v>9</v>
-      </c>
-      <c r="J3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K3" t="s">
-        <v>25</v>
-      </c>
+      <c r="G3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" s="8"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F4" t="s">
         <v>10</v>
       </c>
       <c r="G4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H4" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="I4" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="J4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="63.6" customHeight="1" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="K4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -680,36 +703,33 @@
         <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H5" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="I5" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="J5" t="s">
-        <v>22</v>
-      </c>
-      <c r="K5" s="9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6" t="s">
         <v>15</v>
@@ -724,16 +744,188 @@
         <v>11</v>
       </c>
       <c r="H6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K6" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" t="s">
         <v>26</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I7" t="s">
         <v>26</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J7" t="s">
         <v>27</v>
       </c>
     </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="8">
+        <v>5</v>
+      </c>
+      <c r="B9" s="8">
+        <v>2</v>
+      </c>
+      <c r="C9" s="8">
+        <v>1</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I9" t="s">
+        <v>9</v>
+      </c>
+      <c r="J9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>6</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" t="s">
+        <v>9</v>
+      </c>
+      <c r="I10" t="s">
+        <v>9</v>
+      </c>
+      <c r="J10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>7</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" t="s">
+        <v>26</v>
+      </c>
+      <c r="I11" t="s">
+        <v>26</v>
+      </c>
+      <c r="J11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>8</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" t="s">
+        <v>22</v>
+      </c>
+      <c r="I12" t="s">
+        <v>22</v>
+      </c>
+      <c r="J12" t="s">
+        <v>22</v>
+      </c>
+      <c r="K12" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>9</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" t="s">
+        <v>26</v>
+      </c>
+      <c r="I13" t="s">
+        <v>30</v>
+      </c>
+      <c r="J13" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A8:K8"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>